<commit_message>
created data for national park
</commit_message>
<xml_diff>
--- a/CSV/National Parks.xlsx
+++ b/CSV/National Parks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21943" windowHeight="8091"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Park</t>
   </si>
@@ -77,18 +77,9 @@
     <t>De Soto NATIONAL MEMORIAL</t>
   </si>
   <si>
-    <t>no addy found</t>
-  </si>
-  <si>
     <t>Dry Tortugas NATIONAL PARK</t>
   </si>
   <si>
-    <t>40001 SR-9336</t>
-  </si>
-  <si>
-    <t>Homestead, FL 33034</t>
-  </si>
-  <si>
     <t>Everglades NATIONAL PARK</t>
   </si>
   <si>
@@ -119,29 +110,23 @@
     <t>Gulf Islands NATIONAL SEASHORE</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>Gullah/Geechee CULTURAL HERITAGE CORRIDOR</t>
-  </si>
-  <si>
-    <t>Gullah Geechee Cultural Heritage Corridor</t>
-  </si>
-  <si>
-    <t>2817 Maybank Highway</t>
-  </si>
-  <si>
-    <t>Johns Island, SC 29455</t>
-  </si>
-  <si>
     <t>Timucuan ECOLOGICAL &amp; HISTORIC PRESERVE</t>
+  </si>
+  <si>
+    <t>8300 Desoto Memorial Hwy, Bradenton, FL 34209</t>
+  </si>
+  <si>
+    <t>281 Trumbo Rd, Key West, FL 33040</t>
+  </si>
+  <si>
+    <t>1 Gulf National Sea Shore Dr, Okaloosa Island, FL 32548</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +154,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -200,6 +191,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -481,21 +473,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,33 +501,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="C2">
+        <v>25.857420000000001</v>
+      </c>
+      <c r="D2">
+        <v>-81.033559999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C3">
+        <v>25.464120000000001</v>
+      </c>
+      <c r="D3">
+        <v>-80.336070000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -543,121 +547,155 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="C7">
+        <v>28.92801</v>
+      </c>
+      <c r="D7">
+        <v>-80.823220000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>29.89725</v>
+      </c>
+      <c r="D8">
+        <v>-81.311239999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>27.521350000000002</v>
+      </c>
+      <c r="D10">
+        <v>-82.645020000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>24.56232</v>
+      </c>
+      <c r="D11">
+        <v>-81.798010000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B12" s="1" t="s">
+      <c r="C13">
+        <v>25.395309999999998</v>
+      </c>
+      <c r="D13">
+        <v>-80.583100000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B14" s="1" t="s">
+      <c r="C15">
+        <v>30.383870000000002</v>
+      </c>
+      <c r="D15">
+        <v>-81.499520000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B16" s="1" t="s">
+      <c r="C17">
+        <v>29.86186</v>
+      </c>
+      <c r="D17">
+        <v>-81.280270000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19">
+        <v>30.396830000000001</v>
+      </c>
+      <c r="D19">
+        <v>-86.580520000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>30.383870000000002</v>
+      </c>
+      <c r="D20">
+        <v>-81.499520000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B22" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -670,10 +708,9 @@
     <hyperlink ref="A15" r:id="rId6" display="https://www.nps.gov/foca/"/>
     <hyperlink ref="A17" r:id="rId7" display="https://www.nps.gov/foma/"/>
     <hyperlink ref="A19" r:id="rId8" display="https://www.nps.gov/guis/"/>
-    <hyperlink ref="A20" r:id="rId9" display="https://www.nps.gov/guge/"/>
-    <hyperlink ref="A23" r:id="rId10" display="https://www.nps.gov/timu/"/>
+    <hyperlink ref="A20" r:id="rId9" display="https://www.nps.gov/timu/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>